<commit_message>
First implementation about test cases associated with US1
</commit_message>
<xml_diff>
--- a/test-analysis/test-analysis-template.xlsx
+++ b/test-analysis/test-analysis-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netcompany-my.sharepoint.com/personal/cpapado_netcompany_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serai\Documents\GitHub\Git-Gud-Hackathon\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{E50EEF41-8DF8-4E20-AB0E-1E230EED65DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B15CB03-59D6-4E41-BFEC-1A3646BD91E6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC5FB54-1922-4B47-80BA-D42AE1164BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Report" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -93,13 +93,156 @@
   </si>
   <si>
     <t>Additional comments</t>
+  </si>
+  <si>
+    <t>2a5f45a4-1af5-4cf0-a24d-d87ad4860c9f</t>
+  </si>
+  <si>
+    <t>US1: Add Products in the Cart</t>
+  </si>
+  <si>
+    <t>Verify Product Listing</t>
+  </si>
+  <si>
+    <t>Open the online market and navigate to the fruits section.
+Ensure that all listed products are displayed correctly with their names, prices, and images.
+Verify that the "Add to Cart" button is visible for each product.</t>
+  </si>
+  <si>
+    <t>Have internet connection.</t>
+  </si>
+  <si>
+    <t>e8ac7251-611c-4685-8a5d-9ee53e150678</t>
+  </si>
+  <si>
+    <t>Add Single Product to Cart</t>
+  </si>
+  <si>
+    <t>Select a specific fruit product.</t>
+  </si>
+  <si>
+    <t>Click on the "Add to Cart" button.</t>
+  </si>
+  <si>
+    <t>Confirm that the product is added to the cart.</t>
+  </si>
+  <si>
+    <t>Check that the cart icon displays the correct item count.</t>
+  </si>
+  <si>
+    <t>Add Multiple Products to Cart</t>
+  </si>
+  <si>
+    <t>5f8b88e1-e352-4e29-9c4a-285dd0386ae7</t>
+  </si>
+  <si>
+    <t>Choose different fruit products from the list.</t>
+  </si>
+  <si>
+    <t>Click on the "Add to Cart" button for each selected product.</t>
+  </si>
+  <si>
+    <t>Verify that all selected products are added to the cart.</t>
+  </si>
+  <si>
+    <t>Confirm that the cart icon reflects the accurate total item count.</t>
+  </si>
+  <si>
+    <t>Remove Product from Cart</t>
+  </si>
+  <si>
+    <t>742adf97-198a-4b47-9134-3bab92f3b481</t>
+  </si>
+  <si>
+    <t>Open the online market and navigate to the fruits section.</t>
+  </si>
+  <si>
+    <t>Ensure that all listed products are displayed correctly with their names, prices, and images.</t>
+  </si>
+  <si>
+    <t>Verify that the "Add to Cart" button is visible for each product.</t>
+  </si>
+  <si>
+    <t>Add a product to the cart.</t>
+  </si>
+  <si>
+    <t>Click on the "X" button for the added product.</t>
+  </si>
+  <si>
+    <t>Confirm that the product is successfully removed from the cart.</t>
+  </si>
+  <si>
+    <t>Check that the cart is updated with the correct item count and total price.</t>
+  </si>
+  <si>
+    <t>a7cbf4a5-2e0c-4a8b-be0a-ae72b751f7d3</t>
+  </si>
+  <si>
+    <t>Click the cart icon.</t>
+  </si>
+  <si>
+    <t>Add more of this quantity.</t>
+  </si>
+  <si>
+    <t>Verify that the cart is updated with the correct quantity and total price.</t>
+  </si>
+  <si>
+    <t>b142229b-1c23-4086-b613-869800813345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Product Quantity in Cart </t>
+  </si>
+  <si>
+    <t>Reduce the quantity.</t>
+  </si>
+  <si>
+    <t>Update Product Quantity in Cart by reducing it</t>
+  </si>
+  <si>
+    <t>Cart Summary and Checkout</t>
+  </si>
+  <si>
+    <t>fc49ed79-1a8d-498c-9c7c-090f7b88bd9b</t>
+  </si>
+  <si>
+    <t>Add multiple products to the cart.</t>
+  </si>
+  <si>
+    <t>Go to the cart page and review the summary (product names, quantities, prices).</t>
+  </si>
+  <si>
+    <t>Check that the total price is accurate.</t>
+  </si>
+  <si>
+    <t>Click on the "Proceed to Checkout" button.</t>
+  </si>
+  <si>
+    <t>Verify that the user is directed to the checkout page without errors.</t>
+  </si>
+  <si>
+    <t>Cart Persistence</t>
+  </si>
+  <si>
+    <t>Add products to the cart.</t>
+  </si>
+  <si>
+    <t>Check that the previously added products are still in the cart.</t>
+  </si>
+  <si>
+    <t>Close the browse.</t>
+  </si>
+  <si>
+    <t>Open the online market again.</t>
+  </si>
+  <si>
+    <t>b4441d88-dee4-45a9-9d20-b8713356cf8e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +289,13 @@
       <sz val="10"/>
       <color rgb="FF5E5E5E"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="161"/>
     </font>
   </fonts>
   <fills count="5">
@@ -253,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -270,7 +420,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -281,18 +430,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,18 +439,42 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -329,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,94 +788,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA5E904-0AC9-4BED-A871-AC80F7C33B3B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="26" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="15.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="26" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -729,366 +890,811 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC192840-8274-4346-A7E9-BBD1EE7DFCBA}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="45.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="19"/>
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
-    <row r="10" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A10" s="1" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
+    <row r="11" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="E10" s="4" t="s">
+      <c r="B11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A11" s="7" t="s">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="E11" s="7" t="s">
+      <c r="B12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A12" s="7" t="s">
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="E12" s="7" t="s">
+      <c r="B13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A13" s="7" t="s">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="E13" s="7" t="s">
+      <c r="B14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A14" s="7" t="s">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="E14" s="7" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A15" s="7" t="s">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20"/>
+    </row>
     <row r="19" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A20" s="9"/>
+      <c r="B20" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="12" customHeight="1">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
+    <row r="23" spans="1:6" ht="12" customHeight="1" thickBot="1">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="E19" s="4" t="s">
+      <c r="B23" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A20" s="7" t="s">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1">
+      <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="E20" s="7" t="s">
+      <c r="B24" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="E24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A21" s="7" t="s">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1">
+      <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="E21" s="7" t="s">
+      <c r="B25" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A22" s="7" t="s">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" thickBot="1">
+      <c r="A26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="E22" s="7" t="s">
+      <c r="B26" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="E26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A23" s="7" t="s">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1">
+      <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="E23" s="7" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="E27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A24" s="7" t="s">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" thickBot="1">
+      <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A28" s="1" t="s">
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" thickBot="1">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" thickBot="1"/>
+    <row r="33" spans="1:6" ht="15" thickBot="1">
+      <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="E28" s="4" t="s">
+      <c r="B33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="E33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="7" t="s">
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1">
+      <c r="A34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="E29" s="7" t="s">
+      <c r="B34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="E34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A30" s="7" t="s">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1">
+      <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="E30" s="7" t="s">
+      <c r="B35" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="E35" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A31" s="7" t="s">
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" thickBot="1">
+      <c r="A36" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="E31" s="7" t="s">
+      <c r="B36" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="E36" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A32" s="7" t="s">
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" thickBot="1">
+      <c r="A37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="E32" s="7" t="s">
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+      <c r="E37" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A33" s="7" t="s">
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" thickBot="1">
+      <c r="A38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" thickBot="1">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" thickBot="1">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickBot="1"/>
+    <row r="44" spans="1:6" ht="15" thickBot="1">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" thickBot="1">
+      <c r="A45" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" thickBot="1">
+      <c r="A46" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" thickBot="1">
+      <c r="A47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="17"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" thickBot="1">
+      <c r="A48" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="16"/>
+      <c r="C48" s="17"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1">
+      <c r="A49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" ht="15" thickBot="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" ht="15" thickBot="1">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1"/>
+    <row r="55" spans="1:3" ht="15" thickBot="1">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" ht="15" thickBot="1">
+      <c r="A56" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" ht="15" thickBot="1">
+      <c r="A57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="17"/>
+    </row>
+    <row r="58" spans="1:3" ht="15" thickBot="1">
+      <c r="A58" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="16"/>
+      <c r="C58" s="17"/>
+    </row>
+    <row r="59" spans="1:3" ht="15" thickBot="1">
+      <c r="A59" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="16"/>
+      <c r="C59" s="17"/>
+    </row>
+    <row r="60" spans="1:3" ht="15" thickBot="1">
+      <c r="A60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" thickBot="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" s="9"/>
+    </row>
+    <row r="62" spans="1:3" ht="15" thickBot="1">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="1:3" ht="15" thickBot="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="9"/>
+    </row>
+    <row r="64" spans="1:3" ht="15" thickBot="1">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="9"/>
+    </row>
+    <row r="65" spans="1:3" ht="15" thickBot="1"/>
+    <row r="66" spans="1:3" ht="15" thickBot="1">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" ht="15" thickBot="1">
+      <c r="A67" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" ht="15" thickBot="1">
+      <c r="A68" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="17"/>
+    </row>
+    <row r="69" spans="1:3" ht="15" thickBot="1">
+      <c r="A69" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="16"/>
+      <c r="C69" s="17"/>
+    </row>
+    <row r="70" spans="1:3" ht="15" thickBot="1">
+      <c r="A70" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="16"/>
+      <c r="C70" s="17"/>
+    </row>
+    <row r="71" spans="1:3" ht="15" thickBot="1">
+      <c r="A71" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" thickBot="1">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72" s="9"/>
+    </row>
+    <row r="73" spans="1:3" ht="28.2" thickBot="1">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" s="9"/>
+    </row>
+    <row r="74" spans="1:3" ht="15" thickBot="1">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" s="9"/>
+    </row>
+    <row r="75" spans="1:3" ht="15" thickBot="1">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" s="9"/>
+    </row>
+    <row r="76" spans="1:3" ht="15" thickBot="1">
+      <c r="A76" s="9"/>
+      <c r="B76" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" s="9"/>
+    </row>
+    <row r="77" spans="1:3" ht="15" thickBot="1"/>
+    <row r="78" spans="1:3" ht="15" thickBot="1">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" ht="15" thickBot="1">
+      <c r="A79" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" ht="15" thickBot="1">
+      <c r="A80" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C80" s="17"/>
+    </row>
+    <row r="81" spans="1:3" ht="15" thickBot="1">
+      <c r="A81" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="16"/>
+      <c r="C81" s="17"/>
+    </row>
+    <row r="82" spans="1:3" ht="15" thickBot="1">
+      <c r="A82" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="16"/>
+      <c r="C82" s="17"/>
+    </row>
+    <row r="83" spans="1:3" ht="15" thickBot="1">
+      <c r="A83" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15" thickBot="1">
+      <c r="A84" s="9"/>
+      <c r="B84" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C84" s="9"/>
+    </row>
+    <row r="85" spans="1:3" ht="15" thickBot="1">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C85" s="9"/>
+    </row>
+    <row r="86" spans="1:3" ht="15" thickBot="1">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" s="9"/>
+    </row>
+    <row r="87" spans="1:3" ht="15" thickBot="1">
+      <c r="A87" s="9"/>
+      <c r="B87" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C87" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
+  <mergeCells count="30">
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1103,7 +1709,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1115,7 +1721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1127,7 +1733,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1139,7 +1745,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1153,7 +1759,7 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FIrst impl of Use Case 1 all test cases
</commit_message>
<xml_diff>
--- a/test-analysis/test-analysis-template.xlsx
+++ b/test-analysis/test-analysis-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serai\Documents\GitHub\Git-Gud-Hackathon\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC5FB54-1922-4B47-80BA-D42AE1164BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730D978A-244C-419C-8E85-AA0CD7E90593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -187,18 +187,9 @@
     <t>Verify that the cart is updated with the correct quantity and total price.</t>
   </si>
   <si>
-    <t>b142229b-1c23-4086-b613-869800813345</t>
-  </si>
-  <si>
     <t xml:space="preserve">Update Product Quantity in Cart </t>
   </si>
   <si>
-    <t>Reduce the quantity.</t>
-  </si>
-  <si>
-    <t>Update Product Quantity in Cart by reducing it</t>
-  </si>
-  <si>
     <t>Cart Summary and Checkout</t>
   </si>
   <si>
@@ -217,9 +208,6 @@
     <t>Click on the "Proceed to Checkout" button.</t>
   </si>
   <si>
-    <t>Verify that the user is directed to the checkout page without errors.</t>
-  </si>
-  <si>
     <t>Cart Persistence</t>
   </si>
   <si>
@@ -236,6 +224,21 @@
   </si>
   <si>
     <t>b4441d88-dee4-45a9-9d20-b8713356cf8e</t>
+  </si>
+  <si>
+    <t>A product is already added to the cart</t>
+  </si>
+  <si>
+    <t>cfbacefd-5f82-42ba-9d29-b8f52c5538a2</t>
+  </si>
+  <si>
+    <t>Cart isnt updated</t>
+  </si>
+  <si>
+    <t>If you go to the url /cart instead of clicking procceed to checkout the item number is not updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -324,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -399,11 +402,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF5E5E5E"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF5E5E5E"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -442,6 +456,18 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -460,17 +486,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,30 +820,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="16.2" thickBot="1">
       <c r="A3" s="11"/>
@@ -890,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC192840-8274-4346-A7E9-BBD1EE7DFCBA}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -910,49 +927,55 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="23"/>
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="21"/>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="21"/>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="21"/>
       <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
@@ -962,14 +985,16 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="21"/>
       <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A6" s="6" t="s">
@@ -1012,10 +1037,10 @@
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="23"/>
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1025,10 +1050,10 @@
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="21"/>
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1038,10 +1063,10 @@
       <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="21"/>
       <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1051,10 +1076,10 @@
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="21"/>
       <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1064,8 +1089,8 @@
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
       <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
@@ -1088,52 +1113,52 @@
     </row>
     <row r="17" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="20"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="20"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A19" s="6"/>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="20"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A20" s="9"/>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:6" ht="12" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
     <row r="23" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="19"/>
+      <c r="C23" s="23"/>
       <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
@@ -1143,10 +1168,10 @@
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="21"/>
       <c r="E24" s="6" t="s">
         <v>9</v>
       </c>
@@ -1156,10 +1181,10 @@
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="21"/>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
@@ -1169,10 +1194,10 @@
       <c r="A26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="21"/>
       <c r="E26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1182,8 +1207,8 @@
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
       <c r="E27" s="6" t="s">
         <v>11</v>
       </c>
@@ -1256,10 +1281,10 @@
       <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="21"/>
       <c r="E35" s="6" t="s">
         <v>0</v>
       </c>
@@ -1269,10 +1294,10 @@
       <c r="A36" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="21"/>
       <c r="E36" s="6" t="s">
         <v>10</v>
       </c>
@@ -1282,8 +1307,8 @@
       <c r="A37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
       <c r="E37" s="6" t="s">
         <v>11</v>
       </c>
@@ -1355,24 +1380,26 @@
       <c r="A46" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="17"/>
+      <c r="B46" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="21"/>
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1">
       <c r="A47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
     </row>
     <row r="48" spans="1:6" ht="15" thickBot="1">
       <c r="A48" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+      <c r="B48" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="21"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="6" t="s">
@@ -1413,270 +1440,181 @@
       </c>
       <c r="C53" s="9"/>
     </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1"/>
-    <row r="55" spans="1:3" ht="15" thickBot="1">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:3" ht="15" thickBot="1"/>
+    <row r="56" spans="1:3" ht="15" thickBot="1">
+      <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1">
-      <c r="A56" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C56" s="8"/>
+      <c r="B56" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:3" ht="15" thickBot="1">
       <c r="A57" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1">
       <c r="A58" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="17"/>
+        <v>2</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="21"/>
     </row>
     <row r="59" spans="1:3" ht="15" thickBot="1">
       <c r="A59" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
     </row>
     <row r="60" spans="1:3" ht="15" thickBot="1">
       <c r="A60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="20"/>
+      <c r="C60" s="21"/>
+    </row>
+    <row r="61" spans="1:3" thickBot="1">
+      <c r="A61" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B61" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="15" thickBot="1">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="9"/>
     </row>
     <row r="62" spans="1:3" ht="15" thickBot="1">
       <c r="A62" s="9"/>
       <c r="B62" s="9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C62" s="9"/>
     </row>
-    <row r="63" spans="1:3" ht="15" thickBot="1">
+    <row r="63" spans="1:3" ht="28.2" thickBot="1">
       <c r="A63" s="9"/>
       <c r="B63" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3" ht="15" thickBot="1">
       <c r="A64" s="9"/>
       <c r="B64" s="9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C64" s="9"/>
     </row>
-    <row r="65" spans="1:3" ht="15" thickBot="1"/>
-    <row r="66" spans="1:3" ht="15" thickBot="1">
-      <c r="A66" s="1" t="s">
+    <row r="65" spans="1:4" ht="15" thickBot="1">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" s="9"/>
+    </row>
+    <row r="66" spans="1:4" ht="15" thickBot="1"/>
+    <row r="67" spans="1:4" ht="15" thickBot="1">
+      <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" spans="1:3" ht="15" thickBot="1">
-      <c r="A67" s="6" t="s">
+      <c r="B67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" ht="15" thickBot="1">
+      <c r="A68" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C67" s="8"/>
-    </row>
-    <row r="68" spans="1:3" ht="15" thickBot="1">
-      <c r="A68" s="6" t="s">
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1">
+      <c r="A69" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C68" s="17"/>
-    </row>
-    <row r="69" spans="1:3" ht="15" thickBot="1">
-      <c r="A69" s="6" t="s">
+      <c r="B69" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="21"/>
+    </row>
+    <row r="70" spans="1:4" ht="15" thickBot="1">
+      <c r="A70" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
-    </row>
-    <row r="70" spans="1:3" ht="15" thickBot="1">
-      <c r="A70" s="6" t="s">
+      <c r="B70" s="20"/>
+      <c r="C70" s="21"/>
+    </row>
+    <row r="71" spans="1:4" ht="15" thickBot="1">
+      <c r="A71" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="17"/>
-    </row>
-    <row r="71" spans="1:3" ht="15" thickBot="1">
-      <c r="A71" s="6" t="s">
+      <c r="B71" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="21"/>
+    </row>
+    <row r="72" spans="1:4" ht="15" thickBot="1">
+      <c r="A72" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="15" thickBot="1">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C72" s="9"/>
-    </row>
-    <row r="73" spans="1:3" ht="28.2" thickBot="1">
+      <c r="D72" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" thickBot="1">
       <c r="A73" s="9"/>
       <c r="B73" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C73" s="9"/>
     </row>
-    <row r="74" spans="1:3" ht="15" thickBot="1">
+    <row r="74" spans="1:4" ht="15" thickBot="1">
       <c r="A74" s="9"/>
       <c r="B74" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C74" s="9"/>
     </row>
-    <row r="75" spans="1:3" ht="15" thickBot="1">
+    <row r="75" spans="1:4" ht="15" thickBot="1">
       <c r="A75" s="9"/>
       <c r="B75" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C75" s="9"/>
     </row>
-    <row r="76" spans="1:3" ht="15" thickBot="1">
+    <row r="76" spans="1:4" ht="15" thickBot="1">
       <c r="A76" s="9"/>
       <c r="B76" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C76" s="9"/>
     </row>
-    <row r="77" spans="1:3" ht="15" thickBot="1"/>
-    <row r="78" spans="1:3" ht="15" thickBot="1">
-      <c r="A78" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" spans="1:3" ht="15" thickBot="1">
-      <c r="A79" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" s="8"/>
-    </row>
-    <row r="80" spans="1:3" ht="15" thickBot="1">
-      <c r="A80" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C80" s="17"/>
-    </row>
-    <row r="81" spans="1:3" ht="15" thickBot="1">
-      <c r="A81" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="17"/>
-    </row>
-    <row r="82" spans="1:3" ht="15" thickBot="1">
-      <c r="A82" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="17"/>
-    </row>
-    <row r="83" spans="1:3" ht="15" thickBot="1">
-      <c r="A83" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="15" thickBot="1">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C84" s="9"/>
-    </row>
-    <row r="85" spans="1:3" ht="15" thickBot="1">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C85" s="9"/>
-    </row>
-    <row r="86" spans="1:3" ht="15" thickBot="1">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C86" s="9"/>
-    </row>
-    <row r="87" spans="1:3" ht="15" thickBot="1">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C87" s="9"/>
-    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
+  <mergeCells count="27">
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1689,12 +1627,15 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B69:C69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added US2 test cases
</commit_message>
<xml_diff>
--- a/test-analysis/test-analysis-template.xlsx
+++ b/test-analysis/test-analysis-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netcompany-my.sharepoint.com/personal/cpapado_netcompany_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giannos\VS Code Projects\Git-Gud-Hackathon\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{E50EEF41-8DF8-4E20-AB0E-1E230EED65DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B15CB03-59D6-4E41-BFEC-1A3646BD91E6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A628BC3C-19EE-401D-BF68-D88C3CD6E8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Report" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="57">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -93,6 +93,126 @@
   </si>
   <si>
     <t>Additional comments</t>
+  </si>
+  <si>
+    <t>Verify the redirecton to the "Succesful order" page.</t>
+  </si>
+  <si>
+    <t>Click the "Proceed" button.</t>
+  </si>
+  <si>
+    <t>Seeing the country page.</t>
+  </si>
+  <si>
+    <t>Clicking the "Proceed" button to complete the order.</t>
+  </si>
+  <si>
+    <t>Proceeding to complete the order.</t>
+  </si>
+  <si>
+    <t>US2: Complete Order</t>
+  </si>
+  <si>
+    <t>21bc7390-a029-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Verify that the checkbox is checked.</t>
+  </si>
+  <si>
+    <t>Check the Terms &amp; Conditions checkbox.</t>
+  </si>
+  <si>
+    <t>Checking the Terms &amp; Conditions checkbox.</t>
+  </si>
+  <si>
+    <t>Accept the Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>0658db0c-a029-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Verify that the selected country is displayed.</t>
+  </si>
+  <si>
+    <t>Select the desired country.</t>
+  </si>
+  <si>
+    <t>Open the "Select" dropdown list.</t>
+  </si>
+  <si>
+    <t>Selecting the country from which the order is being placed.</t>
+  </si>
+  <si>
+    <t>Select country</t>
+  </si>
+  <si>
+    <t>ffcc5468-a027-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Verify that the country page is being displayed.</t>
+  </si>
+  <si>
+    <t>Click the "Place Order" button.</t>
+  </si>
+  <si>
+    <t>Seeing the checkout page and the selected items in the cart.</t>
+  </si>
+  <si>
+    <t>Clicking the "Place Order" button and being redirected to the country page.</t>
+  </si>
+  <si>
+    <t>Place order</t>
+  </si>
+  <si>
+    <t>f553548c-a027-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Checkout cart</t>
+  </si>
+  <si>
+    <t>Checkout cart and redirect to the place order page</t>
+  </si>
+  <si>
+    <t>Having products in the cart</t>
+  </si>
+  <si>
+    <t>Click the "Proceed to Checkout" button.</t>
+  </si>
+  <si>
+    <t>Verify that the cart page is being displayed.</t>
+  </si>
+  <si>
+    <t>Verify that all the products are being displayed correctly</t>
+  </si>
+  <si>
+    <t>When placing an order it is possible to proceed without selecting a country.</t>
+  </si>
+  <si>
+    <t>Country selection on order</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>3a00c556-a0af-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Checkout empty cart</t>
+  </si>
+  <si>
+    <t>Make sure the user can not checkout an empty cart</t>
+  </si>
+  <si>
+    <t>Click the "Cart" button</t>
+  </si>
+  <si>
+    <t>See the "Your cart is empty message"</t>
+  </si>
+  <si>
+    <t>"Proceed to checkout" button is faded out</t>
+  </si>
+  <si>
+    <t>28f9caa4-a0b0-11ee-8c90-0242ac120002</t>
   </si>
 </sst>
 </file>
@@ -253,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -270,7 +390,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -281,18 +400,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,14 +409,47 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,94 +767,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA5E904-0AC9-4BED-A871-AC80F7C33B3B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="26" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="15.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="26" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -735,339 +875,338 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="45.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
     <row r="10" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="E11" s="7" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="E11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="E12" s="7" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="E12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="E13" s="7" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="E13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="E14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="12" customHeight="1" thickBot="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="12" customHeight="1" thickBot="1"/>
     <row r="19" spans="1:6" ht="12" customHeight="1" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
       <c r="E19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:6" ht="15" thickBot="1">
+      <c r="A20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="E20" s="7" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="E20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A21" s="7" t="s">
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1">
+      <c r="A21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="E21" s="7" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="E21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A22" s="7" t="s">
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1">
+      <c r="A22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="E22" s="7" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="E22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A23" s="7" t="s">
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="E23" s="7" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="E23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A24" s="7" t="s">
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1">
+      <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" thickBot="1">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1"/>
+    <row r="28" spans="1:6" ht="15" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
       <c r="E28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:6" ht="15" thickBot="1">
+      <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="E29" s="7" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="E29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A30" s="7" t="s">
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1">
+      <c r="A30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="E30" s="7" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="E30" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A31" s="7" t="s">
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" thickBot="1">
+      <c r="A31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="E31" s="7" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="E31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A32" s="7" t="s">
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" thickBot="1">
+      <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="E32" s="7" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="E32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A33" s="7" t="s">
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" thickBot="1">
+      <c r="A33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -1077,11 +1216,6 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1089,6 +1223,11 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1097,14 +1236,577 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242611B2-332F-4034-BDFB-455B2DC6F743}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="F5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1">
+      <c r="A13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1">
+      <c r="A14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1">
+      <c r="A15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1">
+      <c r="A16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="18"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" ht="28.2" thickBot="1">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1"/>
+    <row r="23" spans="1:3" ht="15" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1">
+      <c r="A24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1">
+      <c r="A25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="18"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1">
+      <c r="A26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1">
+      <c r="A27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="18"/>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1">
+      <c r="A28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1"/>
+    <row r="34" spans="1:3" ht="15" thickBot="1">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1">
+      <c r="A35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="24"/>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1">
+      <c r="A36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="18"/>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1">
+      <c r="A37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="26"/>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1">
+      <c r="A38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="18"/>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1">
+      <c r="A39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1"/>
+    <row r="45" spans="1:3" ht="15" thickBot="1">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="22"/>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1">
+      <c r="A46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="24"/>
+    </row>
+    <row r="47" spans="1:3" ht="15" thickBot="1">
+      <c r="A47" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="18"/>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1">
+      <c r="A48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="26"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1">
+      <c r="A49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="18"/>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1">
+      <c r="A50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" thickBot="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" ht="15" thickBot="1">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" ht="15" thickBot="1"/>
+    <row r="56" spans="1:3" ht="15" thickBot="1">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="1:3" ht="15" thickBot="1">
+      <c r="A57" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="24"/>
+    </row>
+    <row r="58" spans="1:3" ht="15" thickBot="1">
+      <c r="A58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" s="18"/>
+    </row>
+    <row r="59" spans="1:3" ht="15" thickBot="1">
+      <c r="A59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="26"/>
+    </row>
+    <row r="60" spans="1:3" ht="15" thickBot="1">
+      <c r="A60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="18"/>
+    </row>
+    <row r="61" spans="1:3" ht="15" thickBot="1">
+      <c r="A61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15" thickBot="1">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="1:3" ht="28.2" thickBot="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="9"/>
+    </row>
+    <row r="64" spans="1:3" ht="15" thickBot="1">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+    </row>
+    <row r="65" spans="1:3" ht="15" thickBot="1">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1115,7 +1817,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1127,7 +1829,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1139,7 +1841,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1153,8 +1855,203 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Έγγραφο" ma:contentTypeID="0x0101008176A71FBDCEC446A54AAA2A3D2C70D7" ma:contentTypeVersion="3" ma:contentTypeDescription="Δημιουργία νέου εγγράφου" ma:contentTypeScope="" ma:versionID="8a699331a0a435e771a067b689ee6b3f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6591812d-8793-43ce-85dc-056ee338b868" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ea3185bad21121e2057fd4289a595d6" ns3:_="">
+    <xsd:import namespace="6591812d-8793-43ce-85dc-056ee338b868"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6591812d-8793-43ce-85dc-056ee338b868" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Τύπος περιεχομένου"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Τίτλος"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{888B36A3-881F-47ED-A2AE-C261F5DCE80B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6591812d-8793-43ce-85dc-056ee338b868"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{226344C0-EE38-4298-A0BC-806596288F1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6591812d-8793-43ce-85dc-056ee338b868"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F96A1B4-AB76-4F29-B828-DEBEE9CAE78E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
US2 test cases change
</commit_message>
<xml_diff>
--- a/test-analysis/test-analysis-template.xlsx
+++ b/test-analysis/test-analysis-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serai\Documents\GitHub\Git-Gud-Hackathon\test-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giannos\VS Code Projects\Git-Gud-Hackathon\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730D978A-244C-419C-8E85-AA0CD7E90593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3104596-221D-4ECF-8181-1B063280093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Report" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="105">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -239,6 +239,126 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>28f9caa4-a0b0-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>US2: Complete Order</t>
+  </si>
+  <si>
+    <t>Checkout empty cart</t>
+  </si>
+  <si>
+    <t>Make sure the user can not checkout an empty cart</t>
+  </si>
+  <si>
+    <t>Country selection on order</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Click the "Cart" button</t>
+  </si>
+  <si>
+    <t>When placing an order it is possible to proceed without selecting a country.</t>
+  </si>
+  <si>
+    <t>See the "Your cart is empty message"</t>
+  </si>
+  <si>
+    <t>"Proceed to checkout" button is faded out</t>
+  </si>
+  <si>
+    <t>3a00c556-a0af-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Checkout cart</t>
+  </si>
+  <si>
+    <t>Checkout cart and redirect to the place order page</t>
+  </si>
+  <si>
+    <t>Having products in the cart</t>
+  </si>
+  <si>
+    <t>Click the "Proceed to Checkout" button.</t>
+  </si>
+  <si>
+    <t>Verify that the cart page is being displayed.</t>
+  </si>
+  <si>
+    <t>Verify that all the products are being displayed correctly</t>
+  </si>
+  <si>
+    <t>f553548c-a027-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Place order</t>
+  </si>
+  <si>
+    <t>Clicking the "Place Order" button and being redirected to the country page.</t>
+  </si>
+  <si>
+    <t>Seeing the checkout page and the selected items in the cart.</t>
+  </si>
+  <si>
+    <t>Click the "Place Order" button.</t>
+  </si>
+  <si>
+    <t>Verify that the country page is being displayed.</t>
+  </si>
+  <si>
+    <t>ffcc5468-a027-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Select country</t>
+  </si>
+  <si>
+    <t>Selecting the country from which the order is being placed.</t>
+  </si>
+  <si>
+    <t>Seeing the country page.</t>
+  </si>
+  <si>
+    <t>Open the "Select" dropdown list.</t>
+  </si>
+  <si>
+    <t>Select the desired country.</t>
+  </si>
+  <si>
+    <t>Verify that the selected country is displayed.</t>
+  </si>
+  <si>
+    <t>0658db0c-a029-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Accept the Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>Checking the Terms &amp; Conditions checkbox.</t>
+  </si>
+  <si>
+    <t>Check the Terms &amp; Conditions checkbox.</t>
+  </si>
+  <si>
+    <t>Verify that the checkbox is checked.</t>
+  </si>
+  <si>
+    <t>21bc7390-a029-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Proceeding to complete the order.</t>
+  </si>
+  <si>
+    <t>Clicking the "Proceed" button to complete the order.</t>
+  </si>
+  <si>
+    <t>Click the "Proceed" button.</t>
+  </si>
+  <si>
+    <t>Verify the redirecton to the "Succesful order" page.</t>
   </si>
 </sst>
 </file>
@@ -417,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -468,6 +588,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -486,12 +609,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -507,7 +648,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -820,30 +961,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="16.2" thickBot="1">
       <c r="A3" s="11"/>
@@ -909,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC192840-8274-4346-A7E9-BBD1EE7DFCBA}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
@@ -927,10 +1068,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="24"/>
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
@@ -942,10 +1083,10 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="22"/>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
@@ -957,10 +1098,10 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="22"/>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
@@ -972,10 +1113,10 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="22"/>
       <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
@@ -985,10 +1126,10 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="22"/>
       <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1037,10 +1178,10 @@
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="24"/>
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1050,10 +1191,10 @@
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1063,10 +1204,10 @@
       <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1076,10 +1217,10 @@
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1089,8 +1230,8 @@
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
@@ -1155,10 +1296,10 @@
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="24"/>
       <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
@@ -1168,10 +1309,10 @@
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="21"/>
+      <c r="C24" s="22"/>
       <c r="E24" s="6" t="s">
         <v>9</v>
       </c>
@@ -1181,10 +1322,10 @@
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="22"/>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
@@ -1194,10 +1335,10 @@
       <c r="A26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="22"/>
       <c r="E26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1207,8 +1348,8 @@
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
       <c r="E27" s="6" t="s">
         <v>11</v>
       </c>
@@ -1281,10 +1422,10 @@
       <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="22"/>
       <c r="E35" s="6" t="s">
         <v>0</v>
       </c>
@@ -1294,10 +1435,10 @@
       <c r="A36" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="22"/>
       <c r="E36" s="6" t="s">
         <v>10</v>
       </c>
@@ -1307,8 +1448,8 @@
       <c r="A37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
       <c r="E37" s="6" t="s">
         <v>11</v>
       </c>
@@ -1380,26 +1521,26 @@
       <c r="A46" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="21"/>
+      <c r="C46" s="22"/>
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1">
       <c r="A47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
     </row>
     <row r="48" spans="1:6" ht="15" thickBot="1">
       <c r="A48" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="21"/>
+      <c r="C48" s="22"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="6" t="s">
@@ -1463,26 +1604,26 @@
       <c r="A58" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="21"/>
+      <c r="C58" s="22"/>
     </row>
     <row r="59" spans="1:3" ht="15" thickBot="1">
       <c r="A59" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="22"/>
     </row>
     <row r="60" spans="1:3" ht="15" thickBot="1">
       <c r="A60" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="21"/>
-    </row>
-    <row r="61" spans="1:3" thickBot="1">
+      <c r="B60" s="21"/>
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="1:3" ht="15" thickBot="1">
       <c r="A61" s="6" t="s">
         <v>5</v>
       </c>
@@ -1544,26 +1685,26 @@
       <c r="A69" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C69" s="21"/>
+      <c r="C69" s="22"/>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1">
       <c r="A70" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="20"/>
-      <c r="C70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="22"/>
     </row>
     <row r="71" spans="1:4" ht="15" thickBot="1">
       <c r="A71" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C71" s="21"/>
+      <c r="C71" s="22"/>
     </row>
     <row r="72" spans="1:4" ht="15" thickBot="1">
       <c r="A72" s="6" t="s">
@@ -1575,7 +1716,7 @@
       <c r="C72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D72" s="18" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1609,12 +1750,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1627,15 +1771,12 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1644,14 +1785,577 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242611B2-332F-4034-BDFB-455B2DC6F743}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="F5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.2" thickBot="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1">
+      <c r="A13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1">
+      <c r="A14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1">
+      <c r="A15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="30"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1">
+      <c r="A16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" ht="28.2" thickBot="1">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1"/>
+    <row r="23" spans="1:3" ht="15" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="26"/>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1">
+      <c r="A24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="28"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1">
+      <c r="A25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="22"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1">
+      <c r="A26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="30"/>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1">
+      <c r="A27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1">
+      <c r="A28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1"/>
+    <row r="34" spans="1:3" ht="15" thickBot="1">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="26"/>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1">
+      <c r="A35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="28"/>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1">
+      <c r="A36" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1">
+      <c r="A37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="30"/>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1">
+      <c r="A38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1">
+      <c r="A39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1"/>
+    <row r="45" spans="1:3" ht="15" thickBot="1">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="26"/>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1">
+      <c r="A46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="28"/>
+    </row>
+    <row r="47" spans="1:3" ht="15" thickBot="1">
+      <c r="A47" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1">
+      <c r="A48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="30"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1">
+      <c r="A49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1">
+      <c r="A50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" thickBot="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" ht="15" thickBot="1">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" ht="15" thickBot="1"/>
+    <row r="56" spans="1:3" ht="15" thickBot="1">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="26"/>
+    </row>
+    <row r="57" spans="1:3" ht="15" thickBot="1">
+      <c r="A57" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="28"/>
+    </row>
+    <row r="58" spans="1:3" ht="15" thickBot="1">
+      <c r="A58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="1:3" ht="15" thickBot="1">
+      <c r="A59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="30"/>
+    </row>
+    <row r="60" spans="1:3" ht="15" thickBot="1">
+      <c r="A60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="1:3" ht="15" thickBot="1">
+      <c r="A61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15" thickBot="1">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="1:3" ht="28.2" thickBot="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="9"/>
+    </row>
+    <row r="64" spans="1:3" ht="15" thickBot="1">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+    </row>
+    <row r="65" spans="1:3" ht="15" thickBot="1">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Finished US2 test cases
</commit_message>
<xml_diff>
--- a/test-analysis/test-analysis-template.xlsx
+++ b/test-analysis/test-analysis-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giannos\VS Code Projects\Git-Gud-Hackathon\test-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3104596-221D-4ECF-8181-1B063280093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D698E7-7957-4C1A-B78A-8918E6190EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{48624885-0AAB-4687-AE04-C5692DDE392F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="115">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -359,6 +359,36 @@
   </si>
   <si>
     <t>Verify the redirecton to the "Succesful order" page.</t>
+  </si>
+  <si>
+    <t>Terms &amp; Conditions checbox not checked</t>
+  </si>
+  <si>
+    <t>Proceeding without checking the T&amp;C checkbox</t>
+  </si>
+  <si>
+    <t>Click the "Proceed" button</t>
+  </si>
+  <si>
+    <t>Display T&amp;C requirement message</t>
+  </si>
+  <si>
+    <t>f97f9b28-a0b4-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>0003bc40-a0b5-11ee-8c90-0242ac120002</t>
+  </si>
+  <si>
+    <t>Block proceeding</t>
+  </si>
+  <si>
+    <t>Do not allow proceeding without a selected country</t>
+  </si>
+  <si>
+    <t>Check the T&amp;B checkbox</t>
+  </si>
+  <si>
+    <t>Display "Country selection required" message</t>
   </si>
 </sst>
 </file>
@@ -591,6 +621,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -625,9 +658,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -961,30 +991,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" ht="16.2" thickBot="1">
       <c r="A3" s="11"/>
@@ -1068,10 +1098,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="25"/>
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1083,10 +1113,10 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1098,10 +1128,10 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="23"/>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1113,10 +1143,10 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
       <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1126,10 +1156,10 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
       <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1178,10 +1208,10 @@
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="25"/>
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1191,10 +1221,10 @@
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="23"/>
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1204,10 +1234,10 @@
       <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="23"/>
       <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1217,10 +1247,10 @@
       <c r="A14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1230,8 +1260,8 @@
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
       <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
@@ -1296,10 +1326,10 @@
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="24"/>
+      <c r="C23" s="25"/>
       <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
@@ -1309,10 +1339,10 @@
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="23"/>
       <c r="E24" s="6" t="s">
         <v>9</v>
       </c>
@@ -1322,10 +1352,10 @@
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="23"/>
       <c r="E25" s="6" t="s">
         <v>0</v>
       </c>
@@ -1335,10 +1365,10 @@
       <c r="A26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="23"/>
       <c r="E26" s="6" t="s">
         <v>10</v>
       </c>
@@ -1348,8 +1378,8 @@
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
       <c r="E27" s="6" t="s">
         <v>11</v>
       </c>
@@ -1422,10 +1452,10 @@
       <c r="A35" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="23"/>
       <c r="E35" s="6" t="s">
         <v>0</v>
       </c>
@@ -1435,10 +1465,10 @@
       <c r="A36" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="23"/>
       <c r="E36" s="6" t="s">
         <v>10</v>
       </c>
@@ -1448,8 +1478,8 @@
       <c r="A37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
       <c r="E37" s="6" t="s">
         <v>11</v>
       </c>
@@ -1521,26 +1551,26 @@
       <c r="A46" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="22"/>
+      <c r="C46" s="23"/>
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1">
       <c r="A47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
     </row>
     <row r="48" spans="1:6" ht="15" thickBot="1">
       <c r="A48" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="22"/>
+      <c r="C48" s="23"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="6" t="s">
@@ -1604,24 +1634,24 @@
       <c r="A58" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="22"/>
+      <c r="C58" s="23"/>
     </row>
     <row r="59" spans="1:3" ht="15" thickBot="1">
       <c r="A59" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="23"/>
     </row>
     <row r="60" spans="1:3" ht="15" thickBot="1">
       <c r="A60" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="22"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="23"/>
     </row>
     <row r="61" spans="1:3" ht="15" thickBot="1">
       <c r="A61" s="6" t="s">
@@ -1685,26 +1715,26 @@
       <c r="A69" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C69" s="22"/>
+      <c r="C69" s="23"/>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1">
       <c r="A70" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
     </row>
     <row r="71" spans="1:4" ht="15" thickBot="1">
       <c r="A71" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C71" s="22"/>
+      <c r="C71" s="23"/>
     </row>
     <row r="72" spans="1:4" ht="15" thickBot="1">
       <c r="A72" s="6" t="s">
@@ -1750,15 +1780,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1771,12 +1798,15 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B69:C69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1785,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242611B2-332F-4034-BDFB-455B2DC6F743}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1804,28 +1834,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="23"/>
       <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1835,10 +1865,10 @@
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="31"/>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1850,8 +1880,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
       <c r="F5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1919,46 +1949,46 @@
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="6" t="s">
@@ -2002,46 +2032,46 @@
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1">
       <c r="A24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1">
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1">
       <c r="A26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="31"/>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1">
       <c r="A27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="23"/>
     </row>
     <row r="28" spans="1:3" ht="15" thickBot="1">
       <c r="A28" s="6" t="s">
@@ -2083,46 +2113,46 @@
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="27"/>
     </row>
     <row r="35" spans="1:3" ht="15" thickBot="1">
       <c r="A35" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:3" ht="15" thickBot="1">
       <c r="A36" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:3" ht="15" thickBot="1">
       <c r="A37" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="30"/>
+      <c r="C37" s="31"/>
     </row>
     <row r="38" spans="1:3" ht="15" thickBot="1">
       <c r="A38" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="23"/>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1">
       <c r="A39" s="6" t="s">
@@ -2166,46 +2196,46 @@
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="26"/>
+      <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:3" ht="15" thickBot="1">
       <c r="A46" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="28"/>
+      <c r="C46" s="29"/>
     </row>
     <row r="47" spans="1:3" ht="15" thickBot="1">
       <c r="A47" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="22"/>
+      <c r="C47" s="23"/>
     </row>
     <row r="48" spans="1:3" ht="15" thickBot="1">
       <c r="A48" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="30"/>
+      <c r="C48" s="31"/>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="22"/>
+      <c r="C49" s="23"/>
     </row>
     <row r="50" spans="1:3" ht="15" thickBot="1">
       <c r="A50" s="6" t="s">
@@ -2242,51 +2272,55 @@
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
     </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1"/>
+    <row r="55" spans="1:3" ht="15" thickBot="1">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+    </row>
     <row r="56" spans="1:3" ht="15" thickBot="1">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="26"/>
+      <c r="B56" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="27"/>
     </row>
     <row r="57" spans="1:3" ht="15" thickBot="1">
       <c r="A57" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C57" s="28"/>
+      <c r="C57" s="29"/>
     </row>
     <row r="58" spans="1:3" ht="15" thickBot="1">
       <c r="A58" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C58" s="22"/>
+      <c r="B58" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="23"/>
     </row>
     <row r="59" spans="1:3" ht="15" thickBot="1">
       <c r="A59" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="30"/>
+      <c r="B59" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="31"/>
     </row>
     <row r="60" spans="1:3" ht="15" thickBot="1">
       <c r="A60" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="22"/>
+      <c r="C60" s="23"/>
     </row>
     <row r="61" spans="1:3" ht="15" thickBot="1">
       <c r="A61" s="6" t="s">
@@ -2302,20 +2336,22 @@
     <row r="62" spans="1:3" ht="15" thickBot="1">
       <c r="A62" s="9"/>
       <c r="B62" s="9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C62" s="9"/>
     </row>
-    <row r="63" spans="1:3" ht="28.2" thickBot="1">
+    <row r="63" spans="1:3" ht="15" thickBot="1">
       <c r="A63" s="9"/>
-      <c r="B63" s="31" t="s">
-        <v>104</v>
+      <c r="B63" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="C63" s="9"/>
     </row>
     <row r="64" spans="1:3" ht="15" thickBot="1">
       <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
+      <c r="B64" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" ht="15" thickBot="1">
@@ -2323,25 +2359,181 @@
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
     </row>
+    <row r="66" spans="1:3" ht="15" thickBot="1">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="27"/>
+    </row>
+    <row r="67" spans="1:3" ht="15" thickBot="1">
+      <c r="A67" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="29"/>
+    </row>
+    <row r="68" spans="1:3" ht="15" thickBot="1">
+      <c r="A68" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="23"/>
+    </row>
+    <row r="69" spans="1:3" ht="15" thickBot="1">
+      <c r="A69" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" s="31"/>
+    </row>
+    <row r="70" spans="1:3" ht="15" thickBot="1">
+      <c r="A70" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="23"/>
+    </row>
+    <row r="71" spans="1:3" ht="15" thickBot="1">
+      <c r="A71" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" thickBot="1">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="9"/>
+    </row>
+    <row r="73" spans="1:3" ht="15" thickBot="1">
+      <c r="A73" s="9"/>
+      <c r="B73" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="9"/>
+    </row>
+    <row r="74" spans="1:3" ht="15" thickBot="1">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="9"/>
+    </row>
+    <row r="75" spans="1:3" ht="15" thickBot="1">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+    </row>
+    <row r="76" spans="1:3" ht="15" thickBot="1"/>
+    <row r="77" spans="1:3" ht="15" thickBot="1">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="27"/>
+    </row>
+    <row r="78" spans="1:3" ht="15" thickBot="1">
+      <c r="A78" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="29"/>
+    </row>
+    <row r="79" spans="1:3" ht="15" thickBot="1">
+      <c r="A79" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="23"/>
+    </row>
+    <row r="80" spans="1:3" ht="15" thickBot="1">
+      <c r="A80" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="31"/>
+    </row>
+    <row r="81" spans="1:3" ht="15" thickBot="1">
+      <c r="A81" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81" s="23"/>
+    </row>
+    <row r="82" spans="1:3" ht="15" thickBot="1">
+      <c r="A82" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" thickBot="1">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" s="9"/>
+    </row>
+    <row r="84" spans="1:3" ht="28.2" thickBot="1">
+      <c r="A84" s="9"/>
+      <c r="B84" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C84" s="9"/>
+    </row>
+    <row r="85" spans="1:3" ht="15" thickBot="1">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+    </row>
+    <row r="86" spans="1:3" ht="15" thickBot="1">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B49:C49"/>
+  <mergeCells count="40">
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -2349,12 +2541,29 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>